<commit_message>
Generated UQ cost units
</commit_message>
<xml_diff>
--- a/validation/cost validation.xlsx
+++ b/validation/cost validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bosoro/Documents/GitHub/saleos/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4C799E-955E-544E-A833-709DDD5B25B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2877E4E-1F35-734D-84C9-30257C696F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="70900" yWindow="500" windowWidth="38480" windowHeight="17440" xr2:uid="{9509160A-B7FD-9E42-B5D6-15488951CEB4}"/>
+    <workbookView xWindow="85080" yWindow="800" windowWidth="38480" windowHeight="22340" xr2:uid="{9509160A-B7FD-9E42-B5D6-15488951CEB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="50">
   <si>
     <t>Parameter</t>
   </si>
@@ -121,18 +121,86 @@
   </si>
   <si>
     <t>Years</t>
+  </si>
+  <si>
+    <t>Regulation Fees Low</t>
+  </si>
+  <si>
+    <t>Regulation Fees High</t>
+  </si>
+  <si>
+    <t>Maintenance Low</t>
+  </si>
+  <si>
+    <t>Maintenance High</t>
+  </si>
+  <si>
+    <t>Staff Low</t>
+  </si>
+  <si>
+    <t>Staff High</t>
+  </si>
+  <si>
+    <t>Subscriber Acquisition Low</t>
+  </si>
+  <si>
+    <t>Subscriber Acquisition High</t>
+  </si>
+  <si>
+    <t>Ground Station Energy Low</t>
+  </si>
+  <si>
+    <t>Ground Station Energy High</t>
+  </si>
+  <si>
+    <t>Fiber Infrastructure Low</t>
+  </si>
+  <si>
+    <t>Fiber Infrastructure High</t>
+  </si>
+  <si>
+    <t>Fiber Length</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>Fiber Length Low</t>
+  </si>
+  <si>
+    <t>Fiber Length High</t>
+  </si>
+  <si>
+    <t>Satellite Manufacturing Low</t>
+  </si>
+  <si>
+    <t>Satellite Launch Low</t>
+  </si>
+  <si>
+    <t>Satellite Manufacturing High</t>
+  </si>
+  <si>
+    <t>Satellite Launch High</t>
+  </si>
+  <si>
+    <t>Ground Station Low</t>
+  </si>
+  <si>
+    <t>Ground Station High</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="172" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="173" formatCode="_(* #,##0.0000000_);_(* \(#,##0.0000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +226,23 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -212,12 +297,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -234,30 +339,71 @@
     <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -573,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9366832D-80E1-234C-9EF7-D348814AE402}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,44 +731,44 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="17.1640625" style="67" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="70" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="62"/>
     <col min="10" max="10" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" style="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="16" t="s">
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
@@ -637,13 +783,13 @@
       <c r="F2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="21" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="14" t="s">
@@ -658,11 +804,11 @@
       <c r="M2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -682,14 +828,14 @@
       <c r="F3" s="4">
         <v>3236</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="63">
         <v>0.4</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="17">
         <f>F3*G3</f>
         <v>1294.4000000000001</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="19">
         <v>648</v>
       </c>
       <c r="J3" s="7">
@@ -705,52 +851,52 @@
       <c r="M3" s="4">
         <v>0.25</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="31">
         <f>L3*M3</f>
         <v>1106.25</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="4">
         <v>19</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="4">
         <v>105</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="23">
         <f>C4*D4</f>
         <v>1995</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="4">
         <v>3236</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="63">
         <v>0.63</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="20">
         <f>F4*G4</f>
         <v>2038.68</v>
       </c>
-      <c r="I4" s="34">
+      <c r="I4" s="22">
         <v>648</v>
       </c>
-      <c r="J4" s="34">
+      <c r="J4" s="25">
         <v>0.1575</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="23">
         <f>I4*J4</f>
         <v>102.06</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="4">
         <v>4425</v>
       </c>
-      <c r="M4" s="30">
+      <c r="M4" s="4">
         <v>0.27300000000000002</v>
       </c>
       <c r="N4" s="31">
@@ -758,47 +904,47 @@
         <v>1208.0250000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="4">
         <v>8</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="4">
         <v>0.5</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="23">
         <f>C5*D5</f>
         <v>4</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="4">
         <v>12</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="63">
         <v>0.5</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="20">
         <f>F5*G5</f>
         <v>6</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="22">
         <v>44</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="25">
         <v>0.5</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="23">
         <f>I5*J5</f>
         <v>22</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="4">
         <v>150</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="4">
         <v>0.5</v>
       </c>
       <c r="N5" s="31">
@@ -806,320 +952,1261 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="47">
         <v>4</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="47">
         <v>0.11758</v>
       </c>
-      <c r="E6" s="31">
-        <f t="shared" ref="E6:E11" si="0">C6*D6</f>
+      <c r="E6" s="23">
+        <f t="shared" ref="E6:E10" si="0">C6*D6</f>
         <v>0.47032000000000002</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="47">
         <v>98</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="53">
         <v>1.2215E-2</v>
       </c>
-      <c r="H6" s="32">
-        <f t="shared" ref="H6:H11" si="1">F6*G6</f>
+      <c r="H6" s="68">
+        <f t="shared" ref="H6:H10" si="1">F6*G6</f>
         <v>1.1970700000000001</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="21">
         <v>100</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="25">
         <v>1.2215E-2</v>
       </c>
-      <c r="K6" s="31">
-        <f t="shared" ref="K6:K11" si="2">I6*J6</f>
+      <c r="K6" s="23">
+        <f t="shared" ref="K6:K10" si="2">I6*J6</f>
         <v>1.2215</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="47">
         <v>190</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="47">
         <v>1.2215E-2</v>
       </c>
-      <c r="N6" s="32">
-        <f t="shared" ref="N6:N11" si="3">L6*M6</f>
+      <c r="N6" s="24">
+        <f t="shared" ref="N6:N10" si="3">L6*M6</f>
         <v>2.3208500000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="O6" s="48">
+        <f>M6*1000000</f>
+        <v>12215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25">
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="20">
         <f>(E11+E5)*0.1</f>
         <v>0.45</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25">
+      <c r="F7" s="47"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="20">
         <f>(H11+H5)*0.1</f>
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="I7" s="26"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="25">
+        <v>0.65250000000000008</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="20">
         <f>(K11+K5)*0.1</f>
         <v>2.4750000000000001</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="25">
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="29">
         <f>(N11+N5)*0.1</f>
         <v>8.4375</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="47">
         <v>2000</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="47">
         <v>0.188</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="23">
         <f t="shared" si="0"/>
         <v>376</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="47">
         <v>1200</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="53">
         <v>0.188</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="20">
         <f t="shared" si="1"/>
         <v>225.6</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="21">
         <v>548</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="25">
         <v>0.188</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="23">
         <f t="shared" si="2"/>
         <v>103.024</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="47">
         <v>2200</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="47">
         <v>0.188</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="28">
         <f t="shared" si="3"/>
         <v>413.6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5">
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="43">
         <v>3.3</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5">
+      <c r="F9" s="42"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="49">
         <v>16</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="5">
+      <c r="I9" s="50"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="43">
         <v>3.3</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="5">
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="31">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="47">
         <v>8</v>
       </c>
-      <c r="D10" s="4">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="D10" s="47">
+        <v>7.6999999999999996E-4</v>
+      </c>
+      <c r="E10" s="23">
         <f t="shared" si="0"/>
-        <v>6.4000000000000003E-3</v>
-      </c>
-      <c r="F10" s="4">
+        <v>6.1599999999999997E-3</v>
+      </c>
+      <c r="F10" s="47">
         <v>12</v>
       </c>
-      <c r="G10" s="4">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="H10" s="5">
+      <c r="G10" s="53">
+        <v>7.6999999999999996E-4</v>
+      </c>
+      <c r="H10" s="20">
         <f t="shared" si="1"/>
-        <v>9.6000000000000009E-3</v>
-      </c>
-      <c r="I10" s="6">
+        <v>9.2399999999999999E-3</v>
+      </c>
+      <c r="I10" s="21">
         <v>44</v>
       </c>
-      <c r="J10" s="10">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="K10" s="5">
+      <c r="J10" s="47">
+        <v>7.6999999999999996E-4</v>
+      </c>
+      <c r="K10" s="23">
         <f t="shared" si="2"/>
-        <v>3.5200000000000002E-2</v>
-      </c>
-      <c r="L10" s="4">
+        <v>3.388E-2</v>
+      </c>
+      <c r="L10" s="47">
         <v>150</v>
       </c>
-      <c r="M10" s="10">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="N10" s="5">
+      <c r="M10" s="47">
+        <v>7.6999999999999996E-4</v>
+      </c>
+      <c r="N10" s="28">
         <f t="shared" si="3"/>
-        <v>0.12000000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.11549999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="4">
         <v>8</v>
       </c>
-      <c r="D11" s="18">
-        <v>6.25E-2</v>
+      <c r="D11" s="16">
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="0"/>
+        <f>D11*C11*C12</f>
         <v>0.5</v>
       </c>
       <c r="F11" s="4">
         <v>12</v>
       </c>
-      <c r="G11" s="4">
-        <v>6.25E-2</v>
-      </c>
-      <c r="H11" s="5">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
-      </c>
-      <c r="I11" s="6">
+      <c r="G11" s="63">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="H11" s="17">
+        <f>G13*F11*G11</f>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I11" s="18">
         <v>44</v>
       </c>
       <c r="J11" s="4">
-        <v>6.25E-2</v>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="K11" s="5">
-        <f t="shared" si="2"/>
+        <f>I12*I11*J11</f>
         <v>2.75</v>
       </c>
       <c r="L11" s="4">
         <v>150</v>
       </c>
       <c r="M11" s="4">
-        <v>6.25E-2</v>
-      </c>
-      <c r="N11" s="5">
-        <f t="shared" si="3"/>
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="N11" s="31">
+        <f>L12*L11*M11</f>
         <v>9.375</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <f>M11*1000000</f>
+        <v>6250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="4">
+        <v>10</v>
+      </c>
+      <c r="G12" s="63"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="18">
+        <v>10</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="4">
+        <v>10</v>
+      </c>
+      <c r="M12" s="4"/>
+      <c r="N12" s="31"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4">
-        <v>7</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4">
-        <v>7</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="7">
-        <v>7</v>
-      </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4">
-        <v>7</v>
-      </c>
-      <c r="N12" s="5"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4">
-        <v>5</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="63">
+        <v>7</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="18"/>
       <c r="J13" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4">
+        <v>7</v>
+      </c>
+      <c r="N13" s="31"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4">
+        <v>15</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="63">
         <v>5</v>
       </c>
-      <c r="N13" s="5"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="7">
+        <v>5</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4">
+        <v>5</v>
+      </c>
+      <c r="N14" s="31"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="37"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B17" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="58"/>
+      <c r="N17" s="58"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="47"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53">
+        <v>19</v>
+      </c>
+      <c r="D19" s="53">
+        <v>200</v>
+      </c>
+      <c r="E19" s="20">
+        <f>D19*C19</f>
+        <v>3800</v>
+      </c>
+      <c r="F19" s="53">
+        <v>3236</v>
+      </c>
+      <c r="G19" s="53">
+        <v>0.3</v>
+      </c>
+      <c r="H19" s="20">
+        <f>G19*F19</f>
+        <v>970.8</v>
+      </c>
+      <c r="I19" s="59">
+        <v>648</v>
+      </c>
+      <c r="J19" s="53">
+        <v>0.3</v>
+      </c>
+      <c r="K19" s="20">
+        <f>J19*I19</f>
+        <v>194.4</v>
+      </c>
+      <c r="L19" s="53">
+        <v>4425</v>
+      </c>
+      <c r="M19" s="53">
+        <v>0.2</v>
+      </c>
+      <c r="N19" s="20">
+        <f>M19*L19</f>
+        <v>885</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53">
+        <v>19</v>
+      </c>
+      <c r="D20" s="53">
+        <v>400</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" ref="E20:E22" si="4">D20*C20</f>
+        <v>7600</v>
+      </c>
+      <c r="F20" s="53">
+        <v>3236</v>
+      </c>
+      <c r="G20" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="20">
+        <f t="shared" ref="H20:H22" si="5">G20*F20</f>
+        <v>1618</v>
+      </c>
+      <c r="I20" s="59">
+        <v>648</v>
+      </c>
+      <c r="J20" s="60">
+        <v>0.5</v>
+      </c>
+      <c r="K20" s="20">
+        <f t="shared" ref="K20:K22" si="6">J20*I20</f>
+        <v>324</v>
+      </c>
+      <c r="L20" s="53">
+        <v>4425</v>
+      </c>
+      <c r="M20" s="53">
+        <v>0.3</v>
+      </c>
+      <c r="N20" s="20">
+        <f>M20*L20</f>
+        <v>1327.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53">
+        <v>19</v>
+      </c>
+      <c r="D21" s="53">
+        <v>80</v>
+      </c>
+      <c r="E21" s="20">
+        <f t="shared" si="4"/>
+        <v>1520</v>
+      </c>
+      <c r="F21" s="53">
+        <v>3236</v>
+      </c>
+      <c r="G21" s="53">
+        <v>0.6</v>
+      </c>
+      <c r="H21" s="20">
+        <f t="shared" si="5"/>
+        <v>1941.6</v>
+      </c>
+      <c r="I21" s="59">
+        <v>648</v>
+      </c>
+      <c r="J21" s="53">
+        <v>0.14749999999999999</v>
+      </c>
+      <c r="K21" s="20">
+        <f t="shared" si="6"/>
+        <v>95.58</v>
+      </c>
+      <c r="L21" s="53">
+        <v>4425</v>
+      </c>
+      <c r="M21" s="53">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="N21" s="20">
+        <f t="shared" ref="N21:N22" si="7">M21*L21</f>
+        <v>1163.7750000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53">
+        <v>19</v>
+      </c>
+      <c r="D22" s="53">
+        <v>130</v>
+      </c>
+      <c r="E22" s="20">
+        <f t="shared" si="4"/>
+        <v>2470</v>
+      </c>
+      <c r="F22" s="53">
+        <v>3236</v>
+      </c>
+      <c r="G22" s="53">
+        <v>0.65</v>
+      </c>
+      <c r="H22" s="20">
+        <f t="shared" si="5"/>
+        <v>2103.4</v>
+      </c>
+      <c r="I22" s="59">
+        <v>648</v>
+      </c>
+      <c r="J22" s="53">
+        <v>0.16750000000000001</v>
+      </c>
+      <c r="K22" s="20">
+        <f t="shared" si="6"/>
+        <v>108.54</v>
+      </c>
+      <c r="L22" s="53">
+        <v>4425</v>
+      </c>
+      <c r="M22" s="53">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="N22" s="20">
+        <f t="shared" si="7"/>
+        <v>1252.2749999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53">
+        <v>8</v>
+      </c>
+      <c r="D23" s="53">
+        <v>0.45</v>
+      </c>
+      <c r="E23" s="20">
+        <f>C23*D23</f>
+        <v>3.6</v>
+      </c>
+      <c r="F23" s="53">
+        <v>12</v>
+      </c>
+      <c r="G23" s="20">
+        <v>0.45</v>
+      </c>
+      <c r="H23" s="20">
+        <f>F23*G23</f>
+        <v>5.4</v>
+      </c>
+      <c r="I23" s="59">
+        <v>44</v>
+      </c>
+      <c r="J23" s="20">
+        <v>0.45</v>
+      </c>
+      <c r="K23" s="20">
+        <f>I23*J23</f>
+        <v>19.8</v>
+      </c>
+      <c r="L23" s="53">
+        <v>150</v>
+      </c>
+      <c r="M23" s="20">
+        <v>0.45</v>
+      </c>
+      <c r="N23" s="20">
+        <f>L23*M23</f>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53">
+        <v>8</v>
+      </c>
+      <c r="D24" s="53">
+        <v>0.6</v>
+      </c>
+      <c r="E24" s="20">
+        <f>C24*D24</f>
+        <v>4.8</v>
+      </c>
+      <c r="F24" s="53">
+        <v>12</v>
+      </c>
+      <c r="G24" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="H24" s="20">
+        <f>F24*G24</f>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="I24" s="59">
+        <v>44</v>
+      </c>
+      <c r="J24" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="K24" s="20">
+        <f>I24*J24</f>
+        <v>26.4</v>
+      </c>
+      <c r="L24" s="53">
+        <v>150</v>
+      </c>
+      <c r="M24" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="N24" s="20">
+        <f>L24*M24</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="47"/>
+      <c r="C25" s="47">
+        <v>4</v>
+      </c>
+      <c r="D25" s="47">
+        <v>0.10758</v>
+      </c>
+      <c r="E25" s="23">
+        <f>C25*D25</f>
+        <v>0.43031999999999998</v>
+      </c>
+      <c r="F25" s="47">
+        <v>98</v>
+      </c>
+      <c r="G25" s="53">
+        <v>1.1214999999999999E-2</v>
+      </c>
+      <c r="H25" s="20">
+        <f>F25*G25</f>
+        <v>1.09907</v>
+      </c>
+      <c r="I25" s="22">
+        <v>100</v>
+      </c>
+      <c r="J25" s="47">
+        <v>1.1214999999999999E-2</v>
+      </c>
+      <c r="K25" s="23">
+        <f>I25*J25</f>
+        <v>1.1214999999999999</v>
+      </c>
+      <c r="L25" s="47">
+        <v>190</v>
+      </c>
+      <c r="M25" s="47">
+        <v>1.1214999999999999E-2</v>
+      </c>
+      <c r="N25" s="23">
+        <f>L25*M25</f>
+        <v>2.1308499999999997</v>
+      </c>
+      <c r="O25">
+        <f>M25*1000000</f>
+        <v>11215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47">
+        <v>4</v>
+      </c>
+      <c r="D26" s="47">
+        <v>0.12758</v>
+      </c>
+      <c r="E26" s="23">
+        <f t="shared" ref="E26:E34" si="8">C26*D26</f>
+        <v>0.51032</v>
+      </c>
+      <c r="F26" s="47">
+        <v>98</v>
+      </c>
+      <c r="G26" s="53">
+        <v>1.3214999999999999E-2</v>
+      </c>
+      <c r="H26" s="20">
+        <f t="shared" ref="H26:H34" si="9">F26*G26</f>
+        <v>1.2950699999999999</v>
+      </c>
+      <c r="I26" s="22">
+        <v>100</v>
+      </c>
+      <c r="J26" s="47">
+        <v>1.3214999999999999E-2</v>
+      </c>
+      <c r="K26" s="23">
+        <f t="shared" ref="K26:K34" si="10">I26*J26</f>
+        <v>1.3214999999999999</v>
+      </c>
+      <c r="L26" s="47">
+        <v>190</v>
+      </c>
+      <c r="M26" s="47">
+        <v>1.3214999999999999E-2</v>
+      </c>
+      <c r="N26" s="23">
+        <f t="shared" ref="N26:N34" si="11">L26*M26</f>
+        <v>2.51085</v>
+      </c>
+      <c r="O26">
+        <f>M26*1000000</f>
+        <v>13215</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="F27" s="47"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="20">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="I27" s="22"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="23">
+        <v>2.38</v>
+      </c>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="23">
+        <v>8.44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="23">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F28" s="47"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="20">
+        <v>0.78</v>
+      </c>
+      <c r="I28" s="22"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="23">
+        <v>2.58</v>
+      </c>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="23">
+        <v>8.34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47">
+        <v>2000</v>
+      </c>
+      <c r="D29" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="E29" s="23">
+        <f t="shared" si="8"/>
+        <v>200</v>
+      </c>
+      <c r="F29" s="47">
+        <v>1200</v>
+      </c>
+      <c r="G29" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="H29" s="20">
+        <f t="shared" si="9"/>
+        <v>120</v>
+      </c>
+      <c r="I29" s="22">
+        <v>548</v>
+      </c>
+      <c r="J29" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="K29" s="23">
+        <f t="shared" si="10"/>
+        <v>54.800000000000004</v>
+      </c>
+      <c r="L29" s="47">
+        <v>2200</v>
+      </c>
+      <c r="M29" s="47">
+        <v>0.1</v>
+      </c>
+      <c r="N29" s="23">
+        <f t="shared" si="11"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47">
+        <v>2000</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="E30" s="23">
+        <f t="shared" si="8"/>
+        <v>500</v>
+      </c>
+      <c r="F30" s="47">
+        <v>1200</v>
+      </c>
+      <c r="G30" s="65">
+        <v>0.25</v>
+      </c>
+      <c r="H30" s="20">
+        <f t="shared" si="9"/>
+        <v>300</v>
+      </c>
+      <c r="I30" s="22">
+        <v>548</v>
+      </c>
+      <c r="J30" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="K30" s="23">
+        <f t="shared" si="10"/>
+        <v>137</v>
+      </c>
+      <c r="L30" s="47">
+        <v>2200</v>
+      </c>
+      <c r="M30" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="N30" s="23">
+        <f t="shared" si="11"/>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="F31" s="47"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="20">
+        <v>15.9</v>
+      </c>
+      <c r="I31" s="22"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="23">
+        <v>3.2</v>
+      </c>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="23">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="23">
+        <v>3.4</v>
+      </c>
+      <c r="F32" s="47"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="20">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="I32" s="22"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="23">
+        <v>3.4</v>
+      </c>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="23">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47">
+        <v>8</v>
+      </c>
+      <c r="D33" s="10">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="E33" s="23">
+        <f t="shared" si="8"/>
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="F33" s="47">
+        <v>12</v>
+      </c>
+      <c r="G33" s="65">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H33" s="20">
+        <f t="shared" si="9"/>
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="I33" s="22">
+        <v>44</v>
+      </c>
+      <c r="J33" s="10">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="K33" s="23">
+        <f t="shared" si="10"/>
+        <v>2.6399999999999996E-2</v>
+      </c>
+      <c r="L33" s="47">
+        <v>150</v>
+      </c>
+      <c r="M33" s="10">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="N33" s="54">
+        <f t="shared" si="11"/>
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47">
+        <v>8</v>
+      </c>
+      <c r="D34" s="10">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="E34" s="23">
+        <f t="shared" si="8"/>
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="F34" s="47">
+        <v>12</v>
+      </c>
+      <c r="G34" s="65">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="H34" s="20">
+        <f t="shared" si="9"/>
+        <v>9.6000000000000009E-3</v>
+      </c>
+      <c r="I34" s="22">
+        <v>44</v>
+      </c>
+      <c r="J34" s="10">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="K34" s="23">
+        <f t="shared" si="10"/>
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="L34" s="47">
+        <v>150</v>
+      </c>
+      <c r="M34" s="10">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="N34" s="54">
+        <f t="shared" si="11"/>
+        <v>0.12000000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="47"/>
+      <c r="C35" s="47">
+        <v>8</v>
+      </c>
+      <c r="D35" s="52">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="E35" s="23">
+        <f>C36*C35*D35</f>
+        <v>0.25</v>
+      </c>
+      <c r="F35" s="47">
+        <v>12</v>
+      </c>
+      <c r="G35" s="66">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="H35" s="20">
+        <f>F36*F35*G35</f>
+        <v>0.375</v>
+      </c>
+      <c r="I35" s="22">
+        <v>44</v>
+      </c>
+      <c r="J35" s="52">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="K35" s="23">
+        <f>I36*I35*J35</f>
+        <v>1.375</v>
+      </c>
+      <c r="L35" s="47">
+        <v>150</v>
+      </c>
+      <c r="M35" s="52">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="N35" s="55">
+        <f>L36*L35*M35</f>
+        <v>4.6875</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="47">
+        <v>5</v>
+      </c>
+      <c r="D36" s="52"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="47">
+        <v>5</v>
+      </c>
+      <c r="G36" s="66"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="22">
+        <v>5</v>
+      </c>
+      <c r="J36" s="52"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="47">
+        <v>5</v>
+      </c>
+      <c r="M36" s="52"/>
+      <c r="N36" s="55"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47">
+        <v>8</v>
+      </c>
+      <c r="D37" s="52">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="E37" s="23">
+        <f>C38*C37*D37</f>
+        <v>0.5</v>
+      </c>
+      <c r="F37" s="47">
+        <v>12</v>
+      </c>
+      <c r="G37" s="66">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="H37" s="20">
+        <f>F38*F37*G37</f>
+        <v>0.75</v>
+      </c>
+      <c r="I37" s="22">
+        <v>44</v>
+      </c>
+      <c r="J37" s="52">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="K37" s="23">
+        <f>I38*I37*J37</f>
+        <v>2.75</v>
+      </c>
+      <c r="L37" s="47">
+        <v>150</v>
+      </c>
+      <c r="M37" s="52">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="N37" s="55">
+        <f>L38*L37*M37</f>
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="57">
+        <v>10</v>
+      </c>
+      <c r="F38" s="57">
+        <v>10</v>
+      </c>
+      <c r="I38" s="60">
+        <v>10</v>
+      </c>
+      <c r="L38" s="57">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="L17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1155,26 +2242,26 @@
       <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="17" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="16" t="s">
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -1408,34 +2495,34 @@
         <v>2.3208500000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="17">
         <f>(E12+E5)*0.1</f>
         <v>0.45</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="17">
         <f>(H12+H5)*0.1</f>
         <v>0.67500000000000004</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="20">
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="17">
         <f>(K12+K5)*0.1</f>
         <v>2.4750000000000001</v>
       </c>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="20">
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="17">
         <f>(N12+N5)*0.1</f>
         <v>8.4375</v>
       </c>
@@ -1622,7 +2709,7 @@
       <c r="C12" s="4">
         <v>8</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>6.25E-2</v>
       </c>
       <c r="E12" s="5">

</xml_diff>

<commit_message>
integrate new uq cost model
</commit_message>
<xml_diff>
--- a/validation/cost validation.xlsx
+++ b/validation/cost validation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bosoro/Documents/GitHub/saleos/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A315AE72-3268-3242-BA67-8CE6A4CD8A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794AB81E-42DD-274E-9773-DA698DF653F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="85080" yWindow="800" windowWidth="38480" windowHeight="22340" xr2:uid="{9509160A-B7FD-9E42-B5D6-15488951CEB4}"/>
+    <workbookView xWindow="59220" yWindow="500" windowWidth="38480" windowHeight="22340" activeTab="1" xr2:uid="{9509160A-B7FD-9E42-B5D6-15488951CEB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="old" sheetId="2" r:id="rId2"/>
+    <sheet name="TCO Calculation" sheetId="3" r:id="rId2"/>
+    <sheet name="old" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="66">
   <si>
     <t>Parameter</t>
   </si>
@@ -187,6 +188,54 @@
   </si>
   <si>
     <t>Ground Station High</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Ground Station</t>
+  </si>
+  <si>
+    <t>Regulation Fees</t>
+  </si>
+  <si>
+    <t>Staff Costs</t>
+  </si>
+  <si>
+    <t>Year 1</t>
+  </si>
+  <si>
+    <t>Year 2</t>
+  </si>
+  <si>
+    <t>Year 3</t>
+  </si>
+  <si>
+    <t>Year 4</t>
+  </si>
+  <si>
+    <t>Year 5</t>
+  </si>
+  <si>
+    <t>US$</t>
+  </si>
+  <si>
+    <t>Capex</t>
+  </si>
+  <si>
+    <t>Opex</t>
+  </si>
+  <si>
+    <t>Total Opex Cost</t>
+  </si>
+  <si>
+    <t>Total Capex Cost</t>
+  </si>
+  <si>
+    <t>Net Present Value of Opex</t>
   </si>
 </sst>
 </file>
@@ -231,6 +280,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,16 +289,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -270,6 +317,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,7 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -355,16 +414,12 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,18 +427,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="172" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="173" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -397,13 +448,20 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -719,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9366832D-80E1-234C-9EF7-D348814AE402}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,16 +789,16 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" style="67" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" style="70" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="62"/>
+    <col min="7" max="7" width="17.1640625" style="58" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="61" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="54"/>
     <col min="10" max="10" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.83203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -768,7 +826,7 @@
       <c r="M1" s="26"/>
       <c r="N1" s="26"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
@@ -783,7 +841,7 @@
       <c r="F2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="55" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="20" t="s">
@@ -804,11 +862,11 @@
       <c r="M2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="N2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -828,7 +886,7 @@
       <c r="F3" s="4">
         <v>3236</v>
       </c>
-      <c r="G3" s="63">
+      <c r="G3" s="55">
         <v>0.4</v>
       </c>
       <c r="H3" s="17">
@@ -851,12 +909,12 @@
       <c r="M3" s="4">
         <v>0.25</v>
       </c>
-      <c r="N3" s="31">
+      <c r="N3" s="23">
         <f>L3*M3</f>
         <v>1106.25</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -876,7 +934,7 @@
       <c r="F4" s="4">
         <v>3236</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="55">
         <v>0.63</v>
       </c>
       <c r="H4" s="20">
@@ -899,12 +957,12 @@
       <c r="M4" s="4">
         <v>0.27300000000000002</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="23">
         <f>L4*M4</f>
         <v>1208.0250000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>21</v>
       </c>
@@ -924,7 +982,7 @@
       <c r="F5" s="4">
         <v>12</v>
       </c>
-      <c r="G5" s="63">
+      <c r="G5" s="55">
         <v>0.5</v>
       </c>
       <c r="H5" s="20">
@@ -947,35 +1005,35 @@
       <c r="M5" s="4">
         <v>0.5</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="23">
         <f>L5*M5</f>
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+    <row r="6" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="39">
         <v>4</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="39">
         <v>0.11758</v>
       </c>
       <c r="E6" s="23">
         <f t="shared" ref="E6:E10" si="0">C6*D6</f>
         <v>0.47032000000000002</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="39">
         <v>98</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="45">
         <v>1.2215E-2</v>
       </c>
-      <c r="H6" s="68">
+      <c r="H6" s="59">
         <f t="shared" ref="H6:H10" si="1">F6*G6</f>
         <v>1.1970700000000001</v>
       </c>
@@ -989,36 +1047,32 @@
         <f t="shared" ref="K6:K10" si="2">I6*J6</f>
         <v>1.2215</v>
       </c>
-      <c r="L6" s="47">
+      <c r="L6" s="39">
         <v>190</v>
       </c>
-      <c r="M6" s="47">
+      <c r="M6" s="39">
         <v>1.2215E-2</v>
       </c>
       <c r="N6" s="24">
         <f t="shared" ref="N6:N10" si="3">L6*M6</f>
         <v>2.3208500000000001</v>
       </c>
-      <c r="O6" s="48">
-        <f>M6*1000000</f>
-        <v>12215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
+    </row>
+    <row r="7" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="20">
         <f>(E11+E5)*0.1</f>
         <v>0.45</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="53"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="20">
         <f>(H11+H5)*0.1</f>
         <v>0.65250000000000008</v>
@@ -1029,34 +1083,34 @@
         <f>(K11+K5)*0.1</f>
         <v>2.4750000000000001</v>
       </c>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="29">
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="20">
         <f>(N11+N5)*0.1</f>
         <v>8.4375</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+    <row r="8" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="39">
         <v>2000</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="39">
         <v>0.188</v>
       </c>
       <c r="E8" s="23">
         <f t="shared" si="0"/>
         <v>376</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="39">
         <v>1200</v>
       </c>
-      <c r="G8" s="53">
+      <c r="G8" s="45">
         <v>0.188</v>
       </c>
       <c r="H8" s="20">
@@ -1073,66 +1127,66 @@
         <f t="shared" si="2"/>
         <v>103.024</v>
       </c>
-      <c r="L8" s="47">
+      <c r="L8" s="39">
         <v>2200</v>
       </c>
-      <c r="M8" s="47">
+      <c r="M8" s="39">
         <v>0.188</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="23">
         <f t="shared" si="3"/>
         <v>413.6</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
+    <row r="9" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43">
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="23">
         <v>3.3</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="49">
+      <c r="F9" s="39"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="20">
         <v>16</v>
       </c>
-      <c r="I9" s="50"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="43">
+      <c r="I9" s="21"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="23">
         <v>3.3</v>
       </c>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="31">
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="23">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+    <row r="10" spans="1:14" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="39">
         <v>8</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="39">
         <v>7.6999999999999996E-4</v>
       </c>
       <c r="E10" s="23">
         <f t="shared" si="0"/>
         <v>6.1599999999999997E-3</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="39">
         <v>12</v>
       </c>
-      <c r="G10" s="53">
+      <c r="G10" s="45">
         <v>7.6999999999999996E-4</v>
       </c>
       <c r="H10" s="20">
@@ -1142,25 +1196,25 @@
       <c r="I10" s="21">
         <v>44</v>
       </c>
-      <c r="J10" s="47">
+      <c r="J10" s="39">
         <v>7.6999999999999996E-4</v>
       </c>
       <c r="K10" s="23">
         <f t="shared" si="2"/>
         <v>3.388E-2</v>
       </c>
-      <c r="L10" s="47">
+      <c r="L10" s="39">
         <v>150</v>
       </c>
-      <c r="M10" s="47">
+      <c r="M10" s="39">
         <v>7.6999999999999996E-4</v>
       </c>
-      <c r="N10" s="28">
+      <c r="N10" s="23">
         <f t="shared" si="3"/>
         <v>0.11549999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>14</v>
       </c>
@@ -1180,7 +1234,7 @@
       <c r="F11" s="4">
         <v>12</v>
       </c>
-      <c r="G11" s="63">
+      <c r="G11" s="55">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="H11" s="17">
@@ -1203,16 +1257,12 @@
       <c r="M11" s="4">
         <v>6.2500000000000003E-3</v>
       </c>
-      <c r="N11" s="31">
+      <c r="N11" s="23">
         <f>L12*L11*M11</f>
         <v>9.375</v>
       </c>
-      <c r="O11">
-        <f>M11*1000000</f>
-        <v>6250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>40</v>
       </c>
@@ -1227,7 +1277,7 @@
       <c r="F12" s="4">
         <v>10</v>
       </c>
-      <c r="G12" s="63"/>
+      <c r="G12" s="55"/>
       <c r="H12" s="17"/>
       <c r="I12" s="18">
         <v>10</v>
@@ -1238,9 +1288,9 @@
         <v>10</v>
       </c>
       <c r="M12" s="4"/>
-      <c r="N12" s="31"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -1253,7 +1303,7 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="63">
+      <c r="G13" s="55">
         <v>7</v>
       </c>
       <c r="H13" s="17"/>
@@ -1266,9 +1316,9 @@
       <c r="M13" s="4">
         <v>7</v>
       </c>
-      <c r="N13" s="31"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
@@ -1281,7 +1331,7 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="63">
+      <c r="G14" s="55">
         <v>5</v>
       </c>
       <c r="H14" s="17"/>
@@ -1294,144 +1344,144 @@
       <c r="M14" s="4">
         <v>5</v>
       </c>
-      <c r="N14" s="31"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="37"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="37"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="38" t="s">
+      <c r="N14" s="23"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="33"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="33"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B17" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39" t="s">
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40" t="s">
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="58" t="s">
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="47"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="51" t="s">
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="39"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="41" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="51" t="s">
+      <c r="F18" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="53" t="s">
+      <c r="G18" s="45" t="s">
         <v>3</v>
       </c>
       <c r="H18" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="59" t="s">
+      <c r="I18" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="J18" s="51" t="s">
+      <c r="J18" s="41" t="s">
         <v>3</v>
       </c>
       <c r="K18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L18" s="51" t="s">
+      <c r="L18" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="51" t="s">
+      <c r="M18" s="41" t="s">
         <v>3</v>
       </c>
       <c r="N18" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="47" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53">
+      <c r="B19" s="45"/>
+      <c r="C19" s="45">
         <v>19</v>
       </c>
-      <c r="D19" s="53">
+      <c r="D19" s="45">
         <v>200</v>
       </c>
       <c r="E19" s="20">
         <f>D19*C19</f>
         <v>3800</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="45">
         <v>3236</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="45">
         <v>0.3</v>
       </c>
       <c r="H19" s="20">
         <f>G19*F19</f>
         <v>970.8</v>
       </c>
-      <c r="I19" s="59">
+      <c r="I19" s="51">
         <v>648</v>
       </c>
-      <c r="J19" s="53">
+      <c r="J19" s="45">
         <v>0.3</v>
       </c>
       <c r="K19" s="20">
         <f>J19*I19</f>
         <v>194.4</v>
       </c>
-      <c r="L19" s="53">
+      <c r="L19" s="45">
         <v>4425</v>
       </c>
-      <c r="M19" s="53">
+      <c r="M19" s="45">
         <v>0.2</v>
       </c>
       <c r="N19" s="20">
@@ -1439,45 +1489,45 @@
         <v>885</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53">
+      <c r="B20" s="45"/>
+      <c r="C20" s="45">
         <v>19</v>
       </c>
-      <c r="D20" s="53">
+      <c r="D20" s="45">
         <v>400</v>
       </c>
       <c r="E20" s="20">
         <f t="shared" ref="E20:E22" si="4">D20*C20</f>
         <v>7600</v>
       </c>
-      <c r="F20" s="53">
+      <c r="F20" s="45">
         <v>3236</v>
       </c>
-      <c r="G20" s="53">
+      <c r="G20" s="45">
         <v>0.5</v>
       </c>
       <c r="H20" s="20">
         <f t="shared" ref="H20:H22" si="5">G20*F20</f>
         <v>1618</v>
       </c>
-      <c r="I20" s="59">
+      <c r="I20" s="51">
         <v>648</v>
       </c>
-      <c r="J20" s="60">
+      <c r="J20" s="52">
         <v>0.5</v>
       </c>
       <c r="K20" s="20">
         <f t="shared" ref="K20:K22" si="6">J20*I20</f>
         <v>324</v>
       </c>
-      <c r="L20" s="53">
+      <c r="L20" s="45">
         <v>4425</v>
       </c>
-      <c r="M20" s="53">
+      <c r="M20" s="45">
         <v>0.3</v>
       </c>
       <c r="N20" s="20">
@@ -1485,45 +1535,45 @@
         <v>1327.5</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="53"/>
-      <c r="C21" s="53">
+      <c r="B21" s="45"/>
+      <c r="C21" s="45">
         <v>19</v>
       </c>
-      <c r="D21" s="53">
+      <c r="D21" s="45">
         <v>80</v>
       </c>
       <c r="E21" s="20">
         <f t="shared" si="4"/>
         <v>1520</v>
       </c>
-      <c r="F21" s="53">
+      <c r="F21" s="45">
         <v>3236</v>
       </c>
-      <c r="G21" s="53">
+      <c r="G21" s="45">
         <v>0.6</v>
       </c>
       <c r="H21" s="20">
         <f t="shared" si="5"/>
         <v>1941.6</v>
       </c>
-      <c r="I21" s="59">
+      <c r="I21" s="51">
         <v>648</v>
       </c>
-      <c r="J21" s="53">
+      <c r="J21" s="45">
         <v>0.14749999999999999</v>
       </c>
       <c r="K21" s="20">
         <f t="shared" si="6"/>
         <v>95.58</v>
       </c>
-      <c r="L21" s="53">
+      <c r="L21" s="45">
         <v>4425</v>
       </c>
-      <c r="M21" s="53">
+      <c r="M21" s="45">
         <v>0.26300000000000001</v>
       </c>
       <c r="N21" s="20">
@@ -1531,45 +1581,45 @@
         <v>1163.7750000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="47" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53">
+      <c r="B22" s="45"/>
+      <c r="C22" s="45">
         <v>19</v>
       </c>
-      <c r="D22" s="53">
+      <c r="D22" s="45">
         <v>130</v>
       </c>
       <c r="E22" s="20">
         <f t="shared" si="4"/>
         <v>2470</v>
       </c>
-      <c r="F22" s="53">
+      <c r="F22" s="45">
         <v>3236</v>
       </c>
-      <c r="G22" s="53">
+      <c r="G22" s="45">
         <v>0.65</v>
       </c>
       <c r="H22" s="20">
         <f t="shared" si="5"/>
         <v>2103.4</v>
       </c>
-      <c r="I22" s="59">
+      <c r="I22" s="51">
         <v>648</v>
       </c>
-      <c r="J22" s="53">
+      <c r="J22" s="45">
         <v>0.16750000000000001</v>
       </c>
       <c r="K22" s="20">
         <f t="shared" si="6"/>
         <v>108.54</v>
       </c>
-      <c r="L22" s="53">
+      <c r="L22" s="45">
         <v>4425</v>
       </c>
-      <c r="M22" s="53">
+      <c r="M22" s="45">
         <v>0.28299999999999997</v>
       </c>
       <c r="N22" s="20">
@@ -1577,22 +1627,22 @@
         <v>1252.2749999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="47" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="53"/>
-      <c r="C23" s="53">
+      <c r="B23" s="45"/>
+      <c r="C23" s="45">
         <v>8</v>
       </c>
-      <c r="D23" s="53">
+      <c r="D23" s="45">
         <v>0.45</v>
       </c>
       <c r="E23" s="20">
         <f>C23*D23</f>
         <v>3.6</v>
       </c>
-      <c r="F23" s="53">
+      <c r="F23" s="45">
         <v>12</v>
       </c>
       <c r="G23" s="20">
@@ -1602,7 +1652,7 @@
         <f>F23*G23</f>
         <v>5.4</v>
       </c>
-      <c r="I23" s="59">
+      <c r="I23" s="51">
         <v>44</v>
       </c>
       <c r="J23" s="20">
@@ -1612,7 +1662,7 @@
         <f>I23*J23</f>
         <v>19.8</v>
       </c>
-      <c r="L23" s="53">
+      <c r="L23" s="45">
         <v>150</v>
       </c>
       <c r="M23" s="20">
@@ -1623,22 +1673,22 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="47" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="53"/>
-      <c r="C24" s="53">
+      <c r="B24" s="45"/>
+      <c r="C24" s="45">
         <v>8</v>
       </c>
-      <c r="D24" s="53">
+      <c r="D24" s="45">
         <v>0.6</v>
       </c>
       <c r="E24" s="20">
         <f>C24*D24</f>
         <v>4.8</v>
       </c>
-      <c r="F24" s="53">
+      <c r="F24" s="45">
         <v>12</v>
       </c>
       <c r="G24" s="20">
@@ -1648,7 +1698,7 @@
         <f>F24*G24</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="I24" s="59">
+      <c r="I24" s="51">
         <v>44</v>
       </c>
       <c r="J24" s="20">
@@ -1658,7 +1708,7 @@
         <f>I24*J24</f>
         <v>26.4</v>
       </c>
-      <c r="L24" s="53">
+      <c r="L24" s="45">
         <v>150</v>
       </c>
       <c r="M24" s="20">
@@ -1669,25 +1719,25 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="46" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="47">
+      <c r="B25" s="39"/>
+      <c r="C25" s="39">
         <v>4</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="39">
         <v>0.10758</v>
       </c>
       <c r="E25" s="23">
         <f>C25*D25</f>
         <v>0.43031999999999998</v>
       </c>
-      <c r="F25" s="47">
+      <c r="F25" s="39">
         <v>98</v>
       </c>
-      <c r="G25" s="53">
+      <c r="G25" s="45">
         <v>1.1214999999999999E-2</v>
       </c>
       <c r="H25" s="20">
@@ -1697,47 +1747,43 @@
       <c r="I25" s="22">
         <v>100</v>
       </c>
-      <c r="J25" s="47">
+      <c r="J25" s="39">
         <v>1.1214999999999999E-2</v>
       </c>
       <c r="K25" s="23">
         <f>I25*J25</f>
         <v>1.1214999999999999</v>
       </c>
-      <c r="L25" s="47">
+      <c r="L25" s="39">
         <v>190</v>
       </c>
-      <c r="M25" s="47">
+      <c r="M25" s="39">
         <v>1.1214999999999999E-2</v>
       </c>
       <c r="N25" s="23">
         <f>L25*M25</f>
         <v>2.1308499999999997</v>
       </c>
-      <c r="O25">
-        <f>M25*1000000</f>
-        <v>11215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="47" t="s">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47">
+      <c r="B26" s="39"/>
+      <c r="C26" s="39">
         <v>4</v>
       </c>
-      <c r="D26" s="47">
+      <c r="D26" s="39">
         <v>0.12758</v>
       </c>
       <c r="E26" s="23">
         <f t="shared" ref="E26:E34" si="8">C26*D26</f>
         <v>0.51032</v>
       </c>
-      <c r="F26" s="47">
+      <c r="F26" s="39">
         <v>98</v>
       </c>
-      <c r="G26" s="53">
+      <c r="G26" s="45">
         <v>1.3214999999999999E-2</v>
       </c>
       <c r="H26" s="20">
@@ -1747,40 +1793,36 @@
       <c r="I26" s="22">
         <v>100</v>
       </c>
-      <c r="J26" s="47">
+      <c r="J26" s="39">
         <v>1.3214999999999999E-2</v>
       </c>
       <c r="K26" s="23">
         <f t="shared" ref="K26:K34" si="10">I26*J26</f>
         <v>1.3214999999999999</v>
       </c>
-      <c r="L26" s="47">
+      <c r="L26" s="39">
         <v>190</v>
       </c>
-      <c r="M26" s="47">
+      <c r="M26" s="39">
         <v>1.3214999999999999E-2</v>
       </c>
       <c r="N26" s="23">
         <f t="shared" ref="N26:N34" si="11">L26*M26</f>
         <v>2.51085</v>
       </c>
-      <c r="O26">
-        <f>M26*1000000</f>
-        <v>13215</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="47" t="s">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
       <c r="E27" s="23">
         <v>0.35</v>
       </c>
-      <c r="F27" s="47"/>
-      <c r="G27" s="53"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="45"/>
       <c r="H27" s="20">
         <v>0.57999999999999996</v>
       </c>
@@ -1789,24 +1831,24 @@
       <c r="K27" s="23">
         <v>2.38</v>
       </c>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
       <c r="N27" s="23">
         <v>8.44</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="47" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="47"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
       <c r="E28" s="23">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F28" s="47"/>
-      <c r="G28" s="53"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="45"/>
       <c r="H28" s="20">
         <v>0.78</v>
       </c>
@@ -1815,31 +1857,31 @@
       <c r="K28" s="23">
         <v>2.58</v>
       </c>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
       <c r="N28" s="23">
         <v>8.34</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="47" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47">
+      <c r="B29" s="39"/>
+      <c r="C29" s="39">
         <v>2000</v>
       </c>
-      <c r="D29" s="47">
+      <c r="D29" s="39">
         <v>0.1</v>
       </c>
       <c r="E29" s="23">
         <f t="shared" si="8"/>
         <v>200</v>
       </c>
-      <c r="F29" s="47">
+      <c r="F29" s="39">
         <v>1200</v>
       </c>
-      <c r="G29" s="53">
+      <c r="G29" s="45">
         <v>0.1</v>
       </c>
       <c r="H29" s="20">
@@ -1849,17 +1891,17 @@
       <c r="I29" s="22">
         <v>548</v>
       </c>
-      <c r="J29" s="47">
+      <c r="J29" s="39">
         <v>0.1</v>
       </c>
       <c r="K29" s="23">
         <f t="shared" si="10"/>
         <v>54.800000000000004</v>
       </c>
-      <c r="L29" s="47">
+      <c r="L29" s="39">
         <v>2200</v>
       </c>
-      <c r="M29" s="47">
+      <c r="M29" s="39">
         <v>0.1</v>
       </c>
       <c r="N29" s="23">
@@ -1867,12 +1909,12 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="47" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47">
+      <c r="B30" s="39"/>
+      <c r="C30" s="39">
         <v>2000</v>
       </c>
       <c r="D30" s="10">
@@ -1882,10 +1924,10 @@
         <f t="shared" si="8"/>
         <v>500</v>
       </c>
-      <c r="F30" s="47">
+      <c r="F30" s="39">
         <v>1200</v>
       </c>
-      <c r="G30" s="65">
+      <c r="G30" s="56">
         <v>0.25</v>
       </c>
       <c r="H30" s="20">
@@ -1902,7 +1944,7 @@
         <f t="shared" si="10"/>
         <v>137</v>
       </c>
-      <c r="L30" s="47">
+      <c r="L30" s="39">
         <v>2200</v>
       </c>
       <c r="M30" s="10">
@@ -1913,18 +1955,18 @@
         <v>550</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="47" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
       <c r="E31" s="23">
         <v>3.2</v>
       </c>
-      <c r="F31" s="47"/>
-      <c r="G31" s="53"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="45"/>
       <c r="H31" s="20">
         <v>15.9</v>
       </c>
@@ -1933,24 +1975,24 @@
       <c r="K31" s="23">
         <v>3.2</v>
       </c>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
       <c r="N31" s="23">
         <v>22.9</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="47" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
-      <c r="D32" s="47"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
       <c r="E32" s="23">
         <v>3.4</v>
       </c>
-      <c r="F32" s="47"/>
-      <c r="G32" s="53"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="45"/>
       <c r="H32" s="20">
         <v>16.100000000000001</v>
       </c>
@@ -1959,18 +2001,18 @@
       <c r="K32" s="23">
         <v>3.4</v>
       </c>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
       <c r="N32" s="23">
         <v>23.1</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47">
+      <c r="B33" s="39"/>
+      <c r="C33" s="39">
         <v>8</v>
       </c>
       <c r="D33" s="10">
@@ -1980,10 +2022,10 @@
         <f t="shared" si="8"/>
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="F33" s="47">
+      <c r="F33" s="39">
         <v>12</v>
       </c>
-      <c r="G33" s="65">
+      <c r="G33" s="56">
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="H33" s="20">
@@ -2000,23 +2042,23 @@
         <f t="shared" si="10"/>
         <v>2.6399999999999996E-2</v>
       </c>
-      <c r="L33" s="47">
+      <c r="L33" s="39">
         <v>150</v>
       </c>
       <c r="M33" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="N33" s="54">
+      <c r="N33" s="46">
         <f t="shared" si="11"/>
         <v>0.09</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="46" t="s">
+      <c r="A34" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47">
+      <c r="B34" s="39"/>
+      <c r="C34" s="39">
         <v>8</v>
       </c>
       <c r="D34" s="10">
@@ -2026,10 +2068,10 @@
         <f t="shared" si="8"/>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="F34" s="47">
+      <c r="F34" s="39">
         <v>12</v>
       </c>
-      <c r="G34" s="65">
+      <c r="G34" s="56">
         <v>8.0000000000000004E-4</v>
       </c>
       <c r="H34" s="20">
@@ -2046,36 +2088,36 @@
         <f t="shared" si="10"/>
         <v>3.5200000000000002E-2</v>
       </c>
-      <c r="L34" s="47">
+      <c r="L34" s="39">
         <v>150</v>
       </c>
       <c r="M34" s="10">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="N34" s="54">
+      <c r="N34" s="46">
         <f t="shared" si="11"/>
         <v>0.12000000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="47">
+      <c r="B35" s="39"/>
+      <c r="C35" s="39">
         <v>8</v>
       </c>
-      <c r="D35" s="52">
+      <c r="D35" s="42">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E35" s="23">
         <f>C36*C35*D35</f>
         <v>0.25</v>
       </c>
-      <c r="F35" s="47">
+      <c r="F35" s="39">
         <v>12</v>
       </c>
-      <c r="G35" s="66">
+      <c r="G35" s="57">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="H35" s="20">
@@ -2085,71 +2127,71 @@
       <c r="I35" s="22">
         <v>44</v>
       </c>
-      <c r="J35" s="52">
+      <c r="J35" s="42">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="K35" s="23">
         <f>I36*I35*J35</f>
         <v>1.375</v>
       </c>
-      <c r="L35" s="47">
+      <c r="L35" s="39">
         <v>150</v>
       </c>
-      <c r="M35" s="52">
+      <c r="M35" s="42">
         <v>6.2500000000000003E-3</v>
       </c>
-      <c r="N35" s="55">
+      <c r="N35" s="47">
         <f>L36*L35*M35</f>
         <v>4.6875</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="47">
+      <c r="C36" s="39">
         <v>5</v>
       </c>
-      <c r="D36" s="52"/>
+      <c r="D36" s="42"/>
       <c r="E36" s="23"/>
-      <c r="F36" s="47">
+      <c r="F36" s="39">
         <v>5</v>
       </c>
-      <c r="G36" s="66"/>
+      <c r="G36" s="57"/>
       <c r="H36" s="20"/>
       <c r="I36" s="22">
         <v>5</v>
       </c>
-      <c r="J36" s="52"/>
+      <c r="J36" s="42"/>
       <c r="K36" s="23"/>
-      <c r="L36" s="47">
+      <c r="L36" s="39">
         <v>5</v>
       </c>
-      <c r="M36" s="52"/>
-      <c r="N36" s="55"/>
+      <c r="M36" s="42"/>
+      <c r="N36" s="47"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47">
+      <c r="B37" s="39"/>
+      <c r="C37" s="39">
         <v>8</v>
       </c>
-      <c r="D37" s="52">
+      <c r="D37" s="42">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="E37" s="23">
         <f>C38*C37*D37</f>
         <v>0.5</v>
       </c>
-      <c r="F37" s="47">
+      <c r="F37" s="39">
         <v>12</v>
       </c>
-      <c r="G37" s="66">
+      <c r="G37" s="57">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="H37" s="20">
@@ -2159,41 +2201,41 @@
       <c r="I37" s="22">
         <v>44</v>
       </c>
-      <c r="J37" s="52">
+      <c r="J37" s="42">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="K37" s="23">
         <f>I38*I37*J37</f>
         <v>2.75</v>
       </c>
-      <c r="L37" s="47">
+      <c r="L37" s="39">
         <v>150</v>
       </c>
-      <c r="M37" s="52">
+      <c r="M37" s="42">
         <v>6.2500000000000003E-3</v>
       </c>
-      <c r="N37" s="55">
+      <c r="N37" s="47">
         <f>L38*L37*M37</f>
         <v>9.375</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="56" t="s">
+      <c r="A38" s="48" t="s">
         <v>43</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="57">
+      <c r="C38" s="49">
         <v>10</v>
       </c>
-      <c r="F38" s="57">
+      <c r="F38" s="49">
         <v>10</v>
       </c>
-      <c r="I38" s="60">
+      <c r="I38" s="52">
         <v>10</v>
       </c>
-      <c r="L38" s="57">
+      <c r="L38" s="49">
         <v>10</v>
       </c>
     </row>
@@ -2213,6 +2255,414 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A627EC-53F7-6F49-82F9-1B1C8E226004}">
+  <dimension ref="A1:AL20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="129" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A2" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1535342250</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A3" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1164509550</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A4" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="5">
+        <v>77017950</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A5" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="5">
+        <v>7062450</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A6" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2467150</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A7" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="5">
+        <v>91500</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A8" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="5">
+        <v>349157600</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A9" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="5">
+        <v>23007841</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A10" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="5">
+        <v>8524170</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A11" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="7">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A12" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="65">
+        <f>SUM(C6:C10)</f>
+        <v>383248261</v>
+      </c>
+      <c r="D13" s="64"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="65">
+        <f>SUM(C2:C6)</f>
+        <v>2786399350</v>
+      </c>
+      <c r="D14" s="64"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="65">
+        <f>SUM(C19:G19)</f>
+        <v>1681391084.6794243</v>
+      </c>
+      <c r="D15" s="64"/>
+    </row>
+    <row r="16" spans="1:38" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="30"/>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="30"/>
+      <c r="AA16" s="30"/>
+      <c r="AB16" s="30"/>
+      <c r="AC16" s="30"/>
+      <c r="AD16" s="30"/>
+      <c r="AE16" s="30"/>
+      <c r="AF16" s="30"/>
+      <c r="AG16" s="30"/>
+      <c r="AH16" s="30"/>
+      <c r="AI16" s="30"/>
+      <c r="AJ16" s="30"/>
+      <c r="AK16" s="30"/>
+      <c r="AL16" s="30"/>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="30"/>
+      <c r="AB17" s="30"/>
+      <c r="AC17" s="30"/>
+      <c r="AD17" s="30"/>
+      <c r="AE17" s="30"/>
+      <c r="AF17" s="30"/>
+      <c r="AG17" s="30"/>
+      <c r="AH17" s="30"/>
+      <c r="AI17" s="30"/>
+      <c r="AJ17" s="30"/>
+      <c r="AK17" s="30"/>
+      <c r="AL17" s="30"/>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="66">
+        <v>0</v>
+      </c>
+      <c r="D18" s="67">
+        <v>1</v>
+      </c>
+      <c r="E18" s="67">
+        <v>2</v>
+      </c>
+      <c r="F18" s="67">
+        <v>3</v>
+      </c>
+      <c r="G18" s="67">
+        <v>4</v>
+      </c>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="30"/>
+      <c r="AA18" s="30"/>
+      <c r="AB18" s="30"/>
+      <c r="AC18" s="30"/>
+      <c r="AD18" s="30"/>
+      <c r="AE18" s="30"/>
+      <c r="AF18" s="30"/>
+      <c r="AG18" s="30"/>
+      <c r="AH18" s="30"/>
+      <c r="AI18" s="30"/>
+      <c r="AJ18" s="30"/>
+      <c r="AK18" s="30"/>
+      <c r="AL18" s="30"/>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="66">
+        <f>C13</f>
+        <v>383248261</v>
+      </c>
+      <c r="D19" s="68">
+        <f>$C$19/POWER(($C$11/100)+1,D18)</f>
+        <v>358175944.85981303</v>
+      </c>
+      <c r="E19" s="68">
+        <f t="shared" ref="E19:G19" si="0">$C$19/POWER(($C$11/100)+1,E18)</f>
+        <v>334743873.70075989</v>
+      </c>
+      <c r="F19" s="68">
+        <f t="shared" si="0"/>
+        <v>312844741.77641112</v>
+      </c>
+      <c r="G19" s="68">
+        <f t="shared" si="0"/>
+        <v>292378263.34244031</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9092088-3647-5E43-A76D-AB8030D3D4FD}">
   <dimension ref="A1:N14"/>
   <sheetViews>

</xml_diff>